<commit_message>
Datadriven test from excel
</commit_message>
<xml_diff>
--- a/web.application/src/test/resources/TestData.xlsx
+++ b/web.application/src/test/resources/TestData.xlsx
@@ -97,8 +97,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>

</xml_diff>